<commit_message>
Pushing stuff for Rev II PCB
</commit_message>
<xml_diff>
--- a/Documentation/Boost MOSFET Dissipation Calcs.xlsx
+++ b/Documentation/Boost MOSFET Dissipation Calcs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents - HDD\KiCad\FusIon Pack\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents - HDD\FusIon Pack\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7656"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -601,26 +601,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="60.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="60.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -632,7 +632,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -645,7 +645,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -677,12 +677,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
         <v>5</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
       </c>
       <c r="C4">
         <v>42</v>
@@ -709,17 +709,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
@@ -732,31 +732,31 @@
       <c r="H7" s="1"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8">
         <f>(C4+H4-A4)/(C4+H4)</f>
-        <v>0.88304093567251463</v>
+        <v>0.53216374269005851</v>
       </c>
       <c r="K8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9">
         <f>B4^2*D4*B8</f>
-        <v>0.11126315789473684</v>
+        <v>0.18625730994152048</v>
       </c>
       <c r="K9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -767,31 +767,31 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12">
         <f>G4-B9</f>
-        <v>1.888736842105263</v>
+        <v>1.8137426900584794</v>
       </c>
       <c r="K12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
       <c r="B13">
         <f>(C4+H4)*B4</f>
-        <v>128.25</v>
+        <v>213.75</v>
       </c>
       <c r="K13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -803,31 +803,31 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
       <c r="B15">
         <f>B13*B14 * (0.000000001)</f>
-        <v>7.1820000000000009E-6</v>
+        <v>1.1970000000000001E-5</v>
       </c>
       <c r="K15" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
       <c r="B16">
         <f>B12/B15</f>
-        <v>262982.01644462027</v>
+        <v>151524.03425718291</v>
       </c>
       <c r="K16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>49</v>
       </c>
@@ -840,37 +840,37 @@
       <c r="H18" s="6"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19">
         <f>G4-B9</f>
-        <v>1.888736842105263</v>
+        <v>1.8137426900584794</v>
       </c>
       <c r="K19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
       <c r="B20">
         <f xml:space="preserve"> 1.7*C4^(1.85)*B4*I4/1000000000000</f>
-        <v>7.9599998857520222E-7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1.3266666476253369E-6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
       <c r="B21">
         <f xml:space="preserve"> B19/B20</f>
-        <v>2372785.0115751908</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1367142.7508221322</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>52</v>
       </c>
@@ -883,37 +883,37 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
       <c r="B24">
         <f>G4-B9</f>
-        <v>1.888736842105263</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1.8137426900584794</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="B25">
         <f xml:space="preserve"> I4/1000000000000*C4^2*B4/F4</f>
-        <v>1.6405200000000001E-6</v>
+        <v>2.7342E-6</v>
       </c>
       <c r="K25" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26">
         <f>B24/B25</f>
-        <v>1151303.758628522</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+        <v>663354.06702453352</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>29</v>
       </c>
@@ -927,7 +927,7 @@
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -935,7 +935,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -943,7 +943,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -951,7 +951,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -959,7 +959,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -967,7 +967,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -975,7 +975,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>37</v>
       </c>
@@ -989,7 +989,7 @@
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -1018,15 +1018,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>20</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C38">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D38">
         <v>0.65</v>
@@ -1035,7 +1035,7 @@
         <v>42</v>
       </c>
       <c r="F38">
-        <v>150000</v>
+        <v>200000</v>
       </c>
       <c r="G38">
         <f>0.84*0.5</f>
@@ -1049,7 +1049,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1058,25 +1058,25 @@
         <v>0.53106682297772567</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41">
         <f>(A38*B40/F38)/(C38/1000000)</f>
-        <v>1.0413074960347561</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1.1299294105909057</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42">
         <f>B41/B38</f>
-        <v>0.52065374801737807</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.37664313686363521</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>56</v>
       </c>
@@ -1091,7 +1091,7 @@
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>5</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>0.55053571106786314</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>5</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>0.82580356660179466</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>9</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>0.69755403565104634</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>9</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>1.0463310534765693</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>15</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>0.81456762037492336</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>15</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>1.2218514305623851</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>20</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>0.84903573423297996</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>20</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>1.2735536013494697</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>20</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>1.6980714684659599</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>20</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>2.1225893355824494</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>57</v>
       </c>
@@ -1501,7 +1501,7 @@
       </c>
       <c r="H57" s="7"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>5</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>9</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>12</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>15</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>20</v>
       </c>

</xml_diff>